<commit_message>
Add dbxls, functions and menuapp
</commit_message>
<xml_diff>
--- a/dbTask.xlsx
+++ b/dbTask.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -519,24 +519,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Tarea c</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>dsajfkl dfsad</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>En espera</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5"/>
     <row r="6"/>
@@ -545,7 +533,6 @@
     <row r="9">
       <c r="J9" s="1" t="n"/>
     </row>
-    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Add flask, index.html, update dbtask
</commit_message>
<xml_diff>
--- a/dbTask.xlsx
+++ b/dbTask.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -484,7 +484,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tarea a</t>
+          <t>Tarea A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>En espera</t>
         </is>
       </c>
     </row>
@@ -518,14 +518,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-    </row>
+    <row r="4"/>
     <row r="5"/>
     <row r="6"/>
     <row r="7"/>
@@ -533,6 +526,7 @@
     <row r="9">
       <c r="J9" s="1" t="n"/>
     </row>
+    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Update db, funciones, add index.html
</commit_message>
<xml_diff>
--- a/dbTask.xlsx
+++ b/dbTask.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -489,12 +489,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>hjashk dflñ</t>
+          <t>Test 2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>En espera</t>
+          <t>En ejecucion</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,6 @@
     <row r="9">
       <c r="J9" s="1" t="n"/>
     </row>
-    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>